<commit_message>
intégration du contenu de la réponse auomatique de contact dans un fichier docx
</commit_message>
<xml_diff>
--- a/data/data_accueil.xlsx
+++ b/data/data_accueil.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dim\clone_repo\portfolio\assets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dim\clone_repo\portfolio\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666A9D39-00B9-44C4-B7CB-28712DA8436F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADF1D75-41A6-4BF5-BD18-D7FE35543AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48AAF2E7-BD52-4126-95BB-1554F7CE70D9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48AAF2E7-BD52-4126-95BB-1554F7CE70D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Nom</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Lefebvre</t>
+  </si>
+  <si>
+    <t>email de communication</t>
+  </si>
+  <si>
+    <t>contact@datadriven-dynamix.fr</t>
   </si>
 </sst>
 </file>
@@ -454,15 +460,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC43A243-20A8-4CB0-8AB2-10C849C7B62F}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="122.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -514,10 +520,19 @@
         <v>6</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{B439D030-0DB2-48D4-9F7F-A2C09BDA55D4}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{FF05D826-F5D2-4D6C-9B72-EFDEA6B262E6}"/>
+    <hyperlink ref="B7" r:id="rId3" xr:uid="{7145CA4F-5CD1-4E25-81B6-BDB90F43445F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modification du menu_hamburger pour utilisation des données depuis data_accueil.xlsx
</commit_message>
<xml_diff>
--- a/data/data_accueil.xlsx
+++ b/data/data_accueil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dim\clone_repo\portfolio\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADF1D75-41A6-4BF5-BD18-D7FE35543AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C16D6F8-F7B5-406C-912B-A06138CA3FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48AAF2E7-BD52-4126-95BB-1554F7CE70D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48AAF2E7-BD52-4126-95BB-1554F7CE70D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -56,28 +56,28 @@
     <t>lien linkedIn</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/dim-lefebvre60</t>
-  </si>
-  <si>
-    <t>https://github.com/Dim2960</t>
-  </si>
-  <si>
-    <t>J’allie expertise technique et vision stratégique pour transformer vos données en performance. Mon expérience passée fait la différence.</t>
-  </si>
-  <si>
-    <t>Data Analyst</t>
-  </si>
-  <si>
-    <t>Dimitri</t>
-  </si>
-  <si>
-    <t>Lefebvre</t>
-  </si>
-  <si>
     <t>email de communication</t>
   </si>
   <si>
     <t>contact@datadriven-dynamix.fr</t>
+  </si>
+  <si>
+    <t>Dimitri1</t>
+  </si>
+  <si>
+    <t>Lefebvre1</t>
+  </si>
+  <si>
+    <t>Data Analyst1</t>
+  </si>
+  <si>
+    <t>https://github.com/Dim29601</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/dim-lefebvre601</t>
+  </si>
+  <si>
+    <t>1J’allie expertise technique et vision stratégique pour transformer vos données en performance. Mon expérience passée fait la différence.</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,18 +474,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -493,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -501,7 +501,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -509,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -517,15 +517,15 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modification du .htaccess pour supp de l'affichage les extensions .php
</commit_message>
<xml_diff>
--- a/data/data_accueil.xlsx
+++ b/data/data_accueil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dim\clone_repo\portfolio\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C16D6F8-F7B5-406C-912B-A06138CA3FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B409103-D1BF-4C7C-8527-6C2DEAA93CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48AAF2E7-BD52-4126-95BB-1554F7CE70D9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48AAF2E7-BD52-4126-95BB-1554F7CE70D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -50,10 +50,22 @@
     <t>Phrase d'accroche</t>
   </si>
   <si>
-    <t>lien github</t>
-  </si>
-  <si>
-    <t>lien linkedIn</t>
+    <t>https://www.linkedin.com/in/dim-lefebvre60</t>
+  </si>
+  <si>
+    <t>https://github.com/Dim2960</t>
+  </si>
+  <si>
+    <t>J’allie expertise technique et vision stratégique pour transformer vos données en performance. Mon expérience passée fait la différence.</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
+  </si>
+  <si>
+    <t>Dimitri</t>
+  </si>
+  <si>
+    <t>Lefebvre</t>
   </si>
   <si>
     <t>email de communication</t>
@@ -62,22 +74,10 @@
     <t>contact@datadriven-dynamix.fr</t>
   </si>
   <si>
-    <t>Dimitri1</t>
-  </si>
-  <si>
-    <t>Lefebvre1</t>
-  </si>
-  <si>
-    <t>Data Analyst1</t>
-  </si>
-  <si>
-    <t>https://github.com/Dim29601</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/dim-lefebvre601</t>
-  </si>
-  <si>
-    <t>1J’allie expertise technique et vision stratégique pour transformer vos données en performance. Mon expérience passée fait la différence.</t>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>LinkedIn</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +493,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -501,31 +501,31 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mise en fonction.php des fonction d extraction des xlsx et docx + correctif affichage bouton mode sombre-clair + correctif envoie mail
</commit_message>
<xml_diff>
--- a/data/data_accueil.xlsx
+++ b/data/data_accueil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dim\clone_repo\portfolio\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B409103-D1BF-4C7C-8527-6C2DEAA93CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCFA148-DB75-45A6-90C8-5CD7058CAC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48AAF2E7-BD52-4126-95BB-1554F7CE70D9}"/>
   </bookViews>
@@ -122,9 +122,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -463,7 +464,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +525,7 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -532,7 +533,6 @@
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{B439D030-0DB2-48D4-9F7F-A2C09BDA55D4}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{FF05D826-F5D2-4D6C-9B72-EFDEA6B262E6}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{7145CA4F-5CD1-4E25-81B6-BDB90F43445F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout de la possibilité de mettre un lien web dans la fiche projet
</commit_message>
<xml_diff>
--- a/data/data_accueil.xlsx
+++ b/data/data_accueil.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dim\clone_repo\portfolio\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FCFA148-DB75-45A6-90C8-5CD7058CAC1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E0CAB8-9507-4D20-A80E-4B2775C37EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48AAF2E7-BD52-4126-95BB-1554F7CE70D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48AAF2E7-BD52-4126-95BB-1554F7CE70D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +96,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,7 +133,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -464,7 +472,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,7 +482,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
@@ -482,7 +490,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -490,7 +498,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -498,7 +506,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -506,7 +514,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -514,7 +522,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -522,10 +530,10 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>